<commit_message>
Adicionado resultado 2 threads
</commit_message>
<xml_diff>
--- a/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
+++ b/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
@@ -242,7 +242,7 @@
   <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0.00" numFmtId="165"/>
-    <numFmt formatCode="0.00%" numFmtId="166"/>
+    <numFmt formatCode="0.000" numFmtId="166"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -276,12 +276,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -318,7 +324,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -327,7 +333,15 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -355,7 +369,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -612,7 +626,7 @@
   <dimension ref="A1:M65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C7" activeCellId="0" pane="topLeft" sqref="C7"/>
+      <selection activeCell="A18" activeCellId="0" pane="topLeft" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -684,8 +698,9 @@
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0</v>
+      <c r="C4" s="2" t="n">
+        <f aca="false">C6*2</f>
+        <v>26897092</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
@@ -709,13 +724,13 @@
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">MAX(C4:G4)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="n">
+        <v>26897092</v>
+      </c>
+      <c r="K4" s="3" t="n">
         <f aca="false">2*K6</f>
         <v>448.284866666667</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="3" t="n">
         <f aca="false">2*L6</f>
         <v>7.47141444444445</v>
       </c>
@@ -754,17 +769,17 @@
         <f aca="false">MAX(C6:G6)</f>
         <v>13448546</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="3" t="n">
         <f aca="false">C6/1000/60</f>
         <v>224.142433333333</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="L6" s="3" t="n">
         <f aca="false">K6/60</f>
         <v>3.73570722222222</v>
       </c>
-      <c r="M6" s="3" t="n">
-        <f aca="false">1 - K6/K4</f>
-        <v>0.5</v>
+      <c r="M6" s="4" t="n">
+        <f aca="false">C4/C6</f>
+        <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
@@ -841,17 +856,17 @@
         <f aca="false">MAX(C10:G10)</f>
         <v>8135505</v>
       </c>
-      <c r="K10" s="2" t="n">
+      <c r="K10" s="3" t="n">
         <f aca="false">C10/1000/60</f>
         <v>135.59175</v>
       </c>
-      <c r="L10" s="2" t="n">
+      <c r="L10" s="3" t="n">
         <f aca="false">K10/60</f>
         <v>2.2598625</v>
       </c>
-      <c r="M10" s="3" t="n">
-        <f aca="false">1 - C10/C6</f>
-        <v>0.395064343758797</v>
+      <c r="M10" s="5" t="n">
+        <f aca="false">C4/C10</f>
+        <v>3.30613674258697</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
@@ -928,17 +943,17 @@
         <f aca="false">MAX(C14:G14)</f>
         <v>5847678</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="K14" s="3" t="n">
         <f aca="false">C14/1000/60</f>
         <v>97.4613</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="L14" s="3" t="n">
         <f aca="false">K14/60</f>
         <v>1.624355</v>
       </c>
-      <c r="M14" s="3" t="n">
-        <f aca="false">1 - C14/C10</f>
-        <v>0.281215118176438</v>
+      <c r="M14" s="5" t="n">
+        <f aca="false">C4/C14</f>
+        <v>4.59961919927876</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">

</xml_diff>

<commit_message>
Gerada primeira imagem de speedup
</commit_message>
<xml_diff>
--- a/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
+++ b/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
@@ -324,7 +324,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -338,10 +338,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -625,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A18" activeCellId="0" pane="topLeft" sqref="A18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B24" activeCellId="0" pane="topLeft" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -699,8 +695,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="n">
-        <f aca="false">C6*2</f>
-        <v>26897092</v>
+        <v>26690977</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
@@ -724,15 +719,19 @@
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">MAX(C4:G4)</f>
-        <v>26897092</v>
+        <v>26690977</v>
       </c>
       <c r="K4" s="3" t="n">
-        <f aca="false">2*K6</f>
-        <v>448.284866666667</v>
+        <f aca="false">C4/1000/60</f>
+        <v>444.849616666667</v>
       </c>
       <c r="L4" s="3" t="n">
-        <f aca="false">2*L6</f>
-        <v>7.47141444444445</v>
+        <f aca="false">K4/60</f>
+        <v>7.41416027777778</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">C4/C4</f>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
@@ -777,9 +776,9 @@
         <f aca="false">K6/60</f>
         <v>3.73570722222222</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="0" t="n">
         <f aca="false">C4/C6</f>
-        <v>2</v>
+        <v>1.98467380785997</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
@@ -864,9 +863,9 @@
         <f aca="false">K10/60</f>
         <v>2.2598625</v>
       </c>
-      <c r="M10" s="5" t="n">
+      <c r="M10" s="4" t="n">
         <f aca="false">C4/C10</f>
-        <v>3.30613674258697</v>
+        <v>3.28080149910792</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
@@ -951,9 +950,9 @@
         <f aca="false">K14/60</f>
         <v>1.624355</v>
       </c>
-      <c r="M14" s="5" t="n">
+      <c r="M14" s="4" t="n">
         <f aca="false">C4/C14</f>
-        <v>4.59961919927876</v>
+        <v>4.5643718754692</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
@@ -1063,6 +1062,17 @@
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>10043951</v>
+      </c>
+      <c r="K22" s="3" t="n">
+        <f aca="false">C22/1000/60</f>
+        <v>167.399183333333</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <f aca="false">K22/60</f>
+        <v>2.78998638888889</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1048576"/>

</xml_diff>

<commit_message>
adicionada curva de evolucao do tempo de execucao
</commit_message>
<xml_diff>
--- a/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
+++ b/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
@@ -318,16 +318,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -616,7 +612,7 @@
   <dimension ref="A1:M65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
+      <selection activeCell="L14" activeCellId="0" pane="topLeft" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -688,11 +684,11 @@
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="0" t="n">
         <v>26690977</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0</v>
+        <v>26628769</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
@@ -705,7 +701,7 @@
       </c>
       <c r="H4" s="0" t="n">
         <f aca="false">(SUM(C4:G4)-J4-I4)/5</f>
-        <v>0</v>
+        <v>5325753.8</v>
       </c>
       <c r="I4" s="0" t="n">
         <f aca="false">MIN(C4:G4)</f>
@@ -715,11 +711,11 @@
         <f aca="false">MAX(C4:G4)</f>
         <v>26690977</v>
       </c>
-      <c r="K4" s="3" t="n">
+      <c r="K4" s="2" t="n">
         <f aca="false">C4/1000/60</f>
         <v>444.849616666667</v>
       </c>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="2" t="n">
         <f aca="false">K4/60</f>
         <v>7.41416027777778</v>
       </c>
@@ -762,15 +758,15 @@
         <f aca="false">MAX(C6:G6)</f>
         <v>13448546</v>
       </c>
-      <c r="K6" s="3" t="n">
+      <c r="K6" s="2" t="n">
         <f aca="false">C6/1000/60</f>
         <v>224.142433333333</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="2" t="n">
         <f aca="false">K6/60</f>
         <v>3.73570722222222</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="3" t="n">
         <f aca="false">C4/C6</f>
         <v>1.98467380785997</v>
       </c>
@@ -849,15 +845,15 @@
         <f aca="false">MAX(C10:G10)</f>
         <v>8135505</v>
       </c>
-      <c r="K10" s="3" t="n">
+      <c r="K10" s="2" t="n">
         <f aca="false">C10/1000/60</f>
         <v>135.59175</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="2" t="n">
         <f aca="false">K10/60</f>
         <v>2.2598625</v>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="M10" s="3" t="n">
         <f aca="false">C4/C10</f>
         <v>3.28080149910792</v>
       </c>
@@ -936,15 +932,15 @@
         <f aca="false">MAX(C14:G14)</f>
         <v>5847678</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="2" t="n">
         <f aca="false">C14/1000/60</f>
         <v>97.4613</v>
       </c>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="2" t="n">
         <f aca="false">K14/60</f>
         <v>1.624355</v>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="M14" s="3" t="n">
         <f aca="false">C4/C14</f>
         <v>4.5643718754692</v>
       </c>
@@ -1060,11 +1056,11 @@
       <c r="C22" s="0" t="n">
         <v>10043951</v>
       </c>
-      <c r="K22" s="3" t="n">
+      <c r="K22" s="2" t="n">
         <f aca="false">C22/1000/60</f>
         <v>167.399183333333</v>
       </c>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="2" t="n">
         <f aca="false">K22/60</f>
         <v>2.78998638888889</v>
       </c>

</xml_diff>

<commit_message>
Adicionado experimento no atilla
</commit_message>
<xml_diff>
--- a/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
+++ b/experiments/dirf_sgsim/DIRFSGS EXPERIMENT HERCULES 256x256x64 - 100 r.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="219" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="131" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -319,7 +319,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -329,10 +329,6 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -618,10 +614,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N65536"/>
+  <dimension ref="A1:O65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
+      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
@@ -735,7 +731,7 @@
         <f aca="false">C4/C4</f>
         <v>1</v>
       </c>
-      <c r="N4" s="3" t="n">
+      <c r="N4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -781,14 +777,15 @@
         <f aca="false">K6/60</f>
         <v>3.73570722222222</v>
       </c>
-      <c r="M6" s="4" t="n">
+      <c r="M6" s="3" t="n">
         <f aca="false">C4/C6</f>
         <v>1.98467380785997</v>
       </c>
-      <c r="N6" s="5" t="n">
+      <c r="N6" s="4" t="n">
         <f aca="false">M6/B6</f>
-        <v>0.992336903929985</v>
-      </c>
+        <v>0.992336903929986</v>
+      </c>
+      <c r="O6" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
@@ -902,14 +899,15 @@
         <f aca="false">K10/60</f>
         <v>2.2598625</v>
       </c>
-      <c r="M10" s="4" t="n">
+      <c r="M10" s="3" t="n">
         <f aca="false">C4/C10</f>
         <v>3.28080149910792</v>
       </c>
-      <c r="N10" s="5" t="n">
+      <c r="N10" s="4" t="n">
         <f aca="false">M10/B10</f>
-        <v>0.82020037477698</v>
-      </c>
+        <v>0.820200374776981</v>
+      </c>
+      <c r="O10" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
@@ -945,6 +943,22 @@
         <f aca="false">MAX(C11:G11)</f>
         <v>0</v>
       </c>
+      <c r="K11" s="2" t="n">
+        <f aca="false">C11/1000/60</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <f aca="false">K11/60</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="3" t="e">
+        <f aca="false">C4/C11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="4" t="e">
+        <f aca="false">M11/B11</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
@@ -954,7 +968,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>0</v>
+        <v>8155605</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0</v>
@@ -978,7 +992,23 @@
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">MAX(C12:G12)</f>
-        <v>0</v>
+        <v>8155605</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <f aca="false">C12/1000/60</f>
+        <v>135.92675</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <f aca="false">K12/60</f>
+        <v>2.26544583333333</v>
+      </c>
+      <c r="M12" s="3" t="n">
+        <f aca="false">C4/C12</f>
+        <v>3.27271575805841</v>
+      </c>
+      <c r="N12" s="4" t="n">
+        <f aca="false">M12/B12</f>
+        <v>0.818178939514604</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
@@ -1023,11 +1053,11 @@
         <f aca="false">K14/60</f>
         <v>1.624355</v>
       </c>
-      <c r="M14" s="4" t="n">
+      <c r="M14" s="3" t="n">
         <f aca="false">C4/C14</f>
         <v>4.5643718754692</v>
       </c>
-      <c r="N14" s="5" t="n">
+      <c r="N14" s="4" t="n">
         <f aca="false">M14/B14</f>
         <v>0.57054648443365</v>
       </c>
@@ -1074,13 +1104,13 @@
         <f aca="false">K15/60</f>
         <v>1.62923694444444</v>
       </c>
-      <c r="M15" s="4" t="n">
+      <c r="M15" s="3" t="n">
         <f aca="false">C4/C15</f>
         <v>4.55069491460982</v>
       </c>
-      <c r="N15" s="5" t="n">
+      <c r="N15" s="4" t="n">
         <f aca="false">M15/B15</f>
-        <v>0.568836864326227</v>
+        <v>0.568836864326228</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
@@ -1125,14 +1155,15 @@
         <f aca="false">K16/60</f>
         <v>1.63273138888889</v>
       </c>
-      <c r="M16" s="4" t="n">
+      <c r="M16" s="3" t="n">
         <f aca="false">C4/C16</f>
         <v>4.54095531465423</v>
       </c>
-      <c r="N16" s="5" t="n">
+      <c r="N16" s="4" t="n">
         <f aca="false">M16/B16</f>
         <v>0.567619414331778</v>
       </c>
+      <c r="O16" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">

</xml_diff>